<commit_message>
change of column name from "mass" to "mass or m/z"
change of column name from "mass" to "mass or m/z"
</commit_message>
<xml_diff>
--- a/files/simulated_theor.xlsx
+++ b/files/simulated_theor.xlsx
@@ -214,7 +214,7 @@
     <t>name</t>
   </si>
   <si>
-    <t>mass</t>
+    <t>mass or m/z</t>
   </si>
 </sst>
 </file>
@@ -581,11 +581,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="12.46484375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">

</xml_diff>